<commit_message>
ResizeRows in closed xml
</commit_message>
<xml_diff>
--- a/src/ExcelsiorClosedXml.Tests/ColumnAttributeTests.Test.verified.xlsx
+++ b/src/ExcelsiorClosedXml.Tests/ColumnAttributeTests.Test.verified.xlsx
@@ -427,7 +427,7 @@
     <x:col min="4" max="4" width="30.710625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:4">
+    <x:row r="1" spans="1:4" ht="14.25" customHeight="1">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -441,7 +441,7 @@
         <x:v>3</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:4">
+    <x:row r="2" spans="1:4" ht="14.25" customHeight="1">
       <x:c r="A2" s="1">
         <x:v>1</x:v>
       </x:c>
@@ -455,7 +455,7 @@
         <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:4">
+    <x:row r="3" spans="1:4" ht="14.25" customHeight="1">
       <x:c r="A3" s="1">
         <x:v>2</x:v>
       </x:c>

</xml_diff>

<commit_message>
Push column width up (#19)
</commit_message>
<xml_diff>
--- a/src/ExcelsiorClosedXml.Tests/ColumnAttributeTests.Test.verified.xlsx
+++ b/src/ExcelsiorClosedXml.Tests/ColumnAttributeTests.Test.verified.xlsx
@@ -421,9 +421,9 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="16.282054" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="15.710625" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="20.710625" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="13.424911" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="12.710625" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="30.710625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>

</xml_diff>